<commit_message>
some updates, removing some unnecessary components
</commit_message>
<xml_diff>
--- a/python/mass_upload/test_dir/test_entry.xlsx
+++ b/python/mass_upload/test_dir/test_entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jon/Documents/2024/idtp/python/mass_upload/test_dir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA579B6-5ACB-544F-A5D0-CBA7D749FFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA54883D-1A73-CD4A-8CF1-B94899F4C6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{D9BB042D-63F3-0843-BBA0-D62D9F429C5E}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="922">
   <si>
     <t>Audio Event (optional)</t>
   </si>
@@ -4869,7 +4869,7 @@
   <dimension ref="A1:AL1040"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5084,7 +5084,7 @@
         <v>915</v>
       </c>
       <c r="E3" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>241</v>
@@ -5160,6 +5160,18 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>

</xml_diff>

<commit_message>
this is all working
</commit_message>
<xml_diff>
--- a/python/mass_upload/test_dir/test_entry.xlsx
+++ b/python/mass_upload/test_dir/test_entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jon/Documents/2024/idtp/python/mass_upload/test_dir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA54883D-1A73-CD4A-8CF1-B94899F4C6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596A1263-2468-CB42-9B47-E49918CE37A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{D9BB042D-63F3-0843-BBA0-D62D9F429C5E}"/>
+    <workbookView xWindow="140" yWindow="760" windowWidth="34240" windowHeight="21260" xr2:uid="{D9BB042D-63F3-0843-BBA0-D62D9F429C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="entries" sheetId="1" r:id="rId1"/>
@@ -4869,7 +4869,7 @@
   <dimension ref="A1:AL1040"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5084,7 +5084,7 @@
         <v>915</v>
       </c>
       <c r="E3" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>241</v>
@@ -5164,7 +5164,7 @@
         <v>915</v>
       </c>
       <c r="E4" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>

</xml_diff>